<commit_message>
Update DTR for John
</commit_message>
<xml_diff>
--- a/DTR/John.xlsx
+++ b/DTR/John.xlsx
@@ -459,6 +459,11 @@
           <t>13:51:48</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>13:52:04</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>